<commit_message>
Ano in ssr, psy-rps, mco, ano out ssr
</commit_message>
<xml_diff>
--- a/formats/excel/MCO/2022/Formats RUM ANO 22.xlsx
+++ b/formats/excel/MCO/2022/Formats RUM ANO 22.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/excel/MCO/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECC7588-A277-984C-873D-25B0D9D91BE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7D92CB-DD7B-8541-85AF-6592DC0CC4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27780" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="258">
   <si>
     <t>nom</t>
   </si>
@@ -779,6 +789,21 @@
   </si>
   <si>
     <t>Zone chiffrée</t>
+  </si>
+  <si>
+    <t>Code retour "identifiant national de santé"</t>
+  </si>
+  <si>
+    <t>Code retour "article 51"</t>
+  </si>
+  <si>
+    <t>ART51</t>
+  </si>
+  <si>
+    <t>CRINS</t>
+  </si>
+  <si>
+    <t>CRART51</t>
   </si>
 </sst>
 </file>
@@ -819,12 +844,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,18 +1124,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="89" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="62.1640625" customWidth="1"/>
-    <col min="5" max="1025" width="9" customWidth="1"/>
+    <col min="5" max="1020" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1690,7 +1712,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>54</v>
       </c>
       <c r="B25">
@@ -2678,8 +2700,8 @@
         <v>136</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B123" si="1">E66+F66-F67</f>
-        <v>0</v>
+        <f>E66+F66-F69</f>
+        <v>-2</v>
       </c>
       <c r="C66" t="s">
         <v>8</v>
@@ -2694,87 +2716,84 @@
         <v>140</v>
       </c>
       <c r="G66" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>256</v>
       </c>
       <c r="B67">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>E67+F67-F70</f>
+        <v>-3</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E67" s="1">
-        <v>2</v>
-      </c>
-      <c r="F67" s="1">
+      <c r="D67" t="s">
+        <v>253</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
         <v>141</v>
       </c>
-      <c r="G67" s="1">
-        <f t="shared" ref="G67:G123" si="2">F67+E67-1</f>
-        <v>142</v>
+      <c r="G67">
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>140</v>
+        <v>257</v>
       </c>
       <c r="B68">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>E68+F68-F71</f>
+        <v>-4</v>
       </c>
       <c r="C68" t="s">
         <v>8</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E68" s="1">
-        <v>2</v>
-      </c>
-      <c r="F68" s="1">
-        <v>143</v>
-      </c>
-      <c r="G68" s="1">
-        <f t="shared" si="2"/>
-        <v>144</v>
+      <c r="D68" t="s">
+        <v>254</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>142</v>
+      </c>
+      <c r="G68">
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B69">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B69:B126" si="1">E69+F69-F70</f>
         <v>0</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
       </c>
       <c r="D69" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E69" s="1">
+        <v>2</v>
+      </c>
+      <c r="F69" s="1">
         <v>143</v>
       </c>
-      <c r="E69" s="1">
-        <v>1</v>
-      </c>
-      <c r="F69" s="1">
-        <v>145</v>
-      </c>
       <c r="G69" s="1">
-        <f t="shared" si="2"/>
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
@@ -2784,22 +2803,21 @@
         <v>8</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E70" s="1">
+        <v>2</v>
+      </c>
+      <c r="F70" s="1">
         <v>145</v>
       </c>
-      <c r="E70" s="1">
-        <v>1</v>
-      </c>
-      <c r="F70" s="1">
-        <v>146</v>
-      </c>
       <c r="G70" s="1">
-        <f t="shared" si="2"/>
         <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B71">
         <f t="shared" si="1"/>
@@ -2809,72 +2827,69 @@
         <v>8</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E71" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" s="1">
         <v>147</v>
       </c>
       <c r="G71" s="1">
-        <f t="shared" si="2"/>
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1">
         <v>148</v>
       </c>
-      <c r="B72">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C72" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E72" s="1">
-        <v>2</v>
-      </c>
-      <c r="F72" s="1">
-        <v>149</v>
-      </c>
       <c r="G72" s="1">
-        <f t="shared" si="2"/>
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E73" s="1">
+        <v>2</v>
+      </c>
+      <c r="F73" s="1">
+        <v>149</v>
+      </c>
+      <c r="G73" s="1">
         <v>150</v>
-      </c>
-      <c r="B73">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C73" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E73" s="1">
-        <v>1</v>
-      </c>
-      <c r="F73" s="1">
-        <v>151</v>
-      </c>
-      <c r="G73" s="1">
-        <f t="shared" si="2"/>
-        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B74">
         <f t="shared" si="1"/>
@@ -2884,22 +2899,21 @@
         <v>8</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E74" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F74" s="1">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G74" s="1">
-        <f t="shared" si="2"/>
         <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B75">
         <f t="shared" si="1"/>
@@ -2909,7 +2923,7 @@
         <v>8</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E75" s="1">
         <v>1</v>
@@ -2918,88 +2932,84 @@
         <v>153</v>
       </c>
       <c r="G75" s="1">
-        <f t="shared" si="2"/>
         <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B76">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C76" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E76" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F76" s="1">
         <v>154</v>
       </c>
       <c r="G76" s="1">
-        <f t="shared" si="2"/>
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B77">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>160</v>
+        <v>8</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E77" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F77" s="1">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G77" s="1">
-        <f t="shared" si="2"/>
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B78">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E78" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F78" s="1">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="G78" s="1">
-        <f t="shared" si="2"/>
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>164</v>
+      <c r="A79" t="s">
+        <v>159</v>
       </c>
       <c r="B79">
         <f t="shared" si="1"/>
@@ -3009,22 +3019,21 @@
         <v>160</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E79" s="1">
         <v>10</v>
       </c>
       <c r="F79" s="1">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="G79" s="1">
-        <f t="shared" si="2"/>
-        <v>187</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B80">
         <f t="shared" si="1"/>
@@ -3034,22 +3043,21 @@
         <v>160</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E80" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F80" s="1">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="G80" s="1">
-        <f t="shared" si="2"/>
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B81">
         <f t="shared" si="1"/>
@@ -3059,22 +3067,21 @@
         <v>160</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E81" s="1">
         <v>10</v>
       </c>
       <c r="F81" s="1">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="G81" s="1">
-        <f t="shared" si="2"/>
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B82">
         <f t="shared" si="1"/>
@@ -3084,72 +3091,69 @@
         <v>160</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E82" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" s="1">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="G82" s="1">
-        <f t="shared" si="2"/>
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B83">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E83" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" s="1">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="G83" s="1">
-        <f t="shared" si="2"/>
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B84">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E84" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F84" s="1">
+        <v>204</v>
+      </c>
+      <c r="G84" s="1">
         <v>208</v>
-      </c>
-      <c r="G84" s="1">
-        <f t="shared" si="2"/>
-        <v>227</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B85">
         <f t="shared" si="1"/>
@@ -3159,22 +3163,21 @@
         <v>8</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E85" s="1">
         <v>1</v>
       </c>
       <c r="F85" s="1">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="G85" s="1">
-        <f t="shared" si="2"/>
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B86">
         <f t="shared" si="1"/>
@@ -3184,22 +3187,21 @@
         <v>8</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E86" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F86" s="1">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="G86" s="1">
-        <f t="shared" si="2"/>
         <v>229</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B87">
         <f t="shared" si="1"/>
@@ -3209,47 +3211,45 @@
         <v>8</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E87" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F87" s="1">
         <v>230</v>
       </c>
       <c r="G87" s="1">
-        <f t="shared" si="2"/>
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B88">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>160</v>
+        <v>8</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E88" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F88" s="1">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G88" s="1">
-        <f t="shared" si="2"/>
-        <v>247</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B89">
         <f t="shared" si="1"/>
@@ -3259,47 +3259,45 @@
         <v>8</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E89" s="1">
         <v>8</v>
       </c>
       <c r="F89" s="1">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G89" s="1">
-        <f t="shared" si="2"/>
-        <v>255</v>
+        <v>239</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B90">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E90" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F90" s="1">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="G90" s="1">
-        <f t="shared" si="2"/>
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B91">
         <f t="shared" si="1"/>
@@ -3309,22 +3307,21 @@
         <v>8</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E91" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F91" s="1">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G91" s="1">
-        <f t="shared" si="2"/>
         <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B92">
         <f t="shared" si="1"/>
@@ -3334,22 +3331,21 @@
         <v>8</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E92" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F92" s="1">
         <v>258</v>
       </c>
       <c r="G92" s="1">
-        <f t="shared" si="2"/>
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B93">
         <f t="shared" si="1"/>
@@ -3359,22 +3355,21 @@
         <v>8</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E93" s="1">
         <v>1</v>
       </c>
       <c r="F93" s="1">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="G93" s="1">
-        <f t="shared" si="2"/>
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B94">
         <f t="shared" si="1"/>
@@ -3384,22 +3379,21 @@
         <v>8</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E94" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F94" s="1">
+        <v>260</v>
+      </c>
+      <c r="G94" s="1">
         <v>268</v>
-      </c>
-      <c r="G94" s="1">
-        <f t="shared" si="2"/>
-        <v>270</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B95">
         <f t="shared" si="1"/>
@@ -3409,22 +3403,21 @@
         <v>8</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E95" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F95" s="1">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G95" s="1">
-        <f t="shared" si="2"/>
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B96">
         <f t="shared" si="1"/>
@@ -3434,22 +3427,21 @@
         <v>8</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E96" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" s="1">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G96" s="1">
-        <f t="shared" si="2"/>
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B97">
         <f t="shared" si="1"/>
@@ -3459,22 +3451,21 @@
         <v>8</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E97" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F97" s="1">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G97" s="1">
-        <f t="shared" si="2"/>
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B98">
         <f t="shared" si="1"/>
@@ -3484,22 +3475,21 @@
         <v>8</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E98" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F98" s="1">
+        <v>276</v>
+      </c>
+      <c r="G98" s="1">
         <v>279</v>
-      </c>
-      <c r="G98" s="1">
-        <f t="shared" si="2"/>
-        <v>287</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B99">
         <f t="shared" si="1"/>
@@ -3509,22 +3499,21 @@
         <v>8</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E99" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F99" s="1">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="G99" s="1">
-        <f t="shared" si="2"/>
-        <v>297</v>
+        <v>280</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B100">
         <f t="shared" si="1"/>
@@ -3534,22 +3523,21 @@
         <v>8</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E100" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F100" s="1">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="G100" s="1">
-        <f t="shared" si="2"/>
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B101">
         <f t="shared" si="1"/>
@@ -3559,22 +3547,21 @@
         <v>8</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E101" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F101" s="1">
+        <v>290</v>
+      </c>
+      <c r="G101" s="1">
         <v>299</v>
-      </c>
-      <c r="G101" s="1">
-        <f t="shared" si="2"/>
-        <v>306</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B102">
         <f t="shared" si="1"/>
@@ -3584,22 +3571,21 @@
         <v>8</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E102" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F102" s="1">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="G102" s="1">
-        <f t="shared" si="2"/>
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B103">
         <f t="shared" si="1"/>
@@ -3609,22 +3595,21 @@
         <v>8</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E103" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F103" s="1">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="G103" s="1">
-        <f t="shared" si="2"/>
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B104">
         <f t="shared" si="1"/>
@@ -3634,22 +3619,21 @@
         <v>8</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E104" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F104" s="1">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="G104" s="1">
-        <f t="shared" si="2"/>
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B105">
         <f t="shared" si="1"/>
@@ -3659,22 +3643,21 @@
         <v>8</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E105" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F105" s="1">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G105" s="1">
-        <f t="shared" si="2"/>
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B106">
         <f t="shared" si="1"/>
@@ -3684,22 +3667,21 @@
         <v>8</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E106" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F106" s="1">
+        <v>320</v>
+      </c>
+      <c r="G106" s="1">
         <v>322</v>
-      </c>
-      <c r="G106" s="1">
-        <f t="shared" si="2"/>
-        <v>329</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B107">
         <f t="shared" si="1"/>
@@ -3709,47 +3691,45 @@
         <v>8</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E107" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F107" s="1">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="G107" s="1">
-        <f t="shared" si="2"/>
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B108">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C108" t="s">
-        <v>160</v>
+        <v>8</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E108" s="1">
         <v>8</v>
       </c>
       <c r="F108" s="1">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="G108" s="1">
-        <f t="shared" si="2"/>
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B109">
         <f t="shared" si="1"/>
@@ -3759,47 +3739,45 @@
         <v>8</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E109" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F109" s="1">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="G109" s="1">
-        <f t="shared" si="2"/>
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B110">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C110" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E110" s="1">
         <v>8</v>
       </c>
       <c r="F110" s="1">
+        <v>340</v>
+      </c>
+      <c r="G110" s="1">
         <v>347</v>
-      </c>
-      <c r="G110" s="1">
-        <f t="shared" si="2"/>
-        <v>354</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B111">
         <f t="shared" si="1"/>
@@ -3809,22 +3787,21 @@
         <v>8</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E111" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F111" s="1">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="G111" s="1">
-        <f t="shared" si="2"/>
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B112">
         <f t="shared" si="1"/>
@@ -3834,22 +3811,21 @@
         <v>8</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E112" s="1">
         <v>8</v>
       </c>
       <c r="F112" s="1">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="G112" s="1">
-        <f t="shared" si="2"/>
-        <v>370</v>
+        <v>356</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B113">
         <f t="shared" si="1"/>
@@ -3859,22 +3835,21 @@
         <v>8</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E113" s="1">
         <v>8</v>
       </c>
       <c r="F113" s="1">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="G113" s="1">
-        <f t="shared" si="2"/>
-        <v>378</v>
+        <v>364</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B114">
         <f t="shared" si="1"/>
@@ -3884,22 +3859,21 @@
         <v>8</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E114" s="1">
         <v>8</v>
       </c>
       <c r="F114" s="1">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="G114" s="1">
-        <f t="shared" si="2"/>
-        <v>386</v>
+        <v>372</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B115">
         <f t="shared" si="1"/>
@@ -3909,22 +3883,21 @@
         <v>8</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E115" s="1">
         <v>8</v>
       </c>
       <c r="F115" s="1">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="G115" s="1">
-        <f t="shared" si="2"/>
-        <v>394</v>
+        <v>380</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B116">
         <f t="shared" si="1"/>
@@ -3934,22 +3907,21 @@
         <v>8</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E116" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F116" s="1">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="G116" s="1">
-        <f t="shared" si="2"/>
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B117">
         <f t="shared" si="1"/>
@@ -3959,22 +3931,21 @@
         <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E117" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F117" s="1">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G117" s="1">
-        <f t="shared" si="2"/>
         <v>396</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B118">
         <f t="shared" si="1"/>
@@ -3984,7 +3955,7 @@
         <v>8</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E118" s="1">
         <v>1</v>
@@ -3993,13 +3964,12 @@
         <v>397</v>
       </c>
       <c r="G118" s="1">
-        <f t="shared" si="2"/>
         <v>397</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B119">
         <f t="shared" si="1"/>
@@ -4009,22 +3979,21 @@
         <v>8</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E119" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F119" s="1">
         <v>398</v>
       </c>
       <c r="G119" s="1">
-        <f t="shared" si="2"/>
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B120">
         <f t="shared" si="1"/>
@@ -4034,22 +4003,21 @@
         <v>8</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E120" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F120" s="1">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G120" s="1">
-        <f t="shared" si="2"/>
-        <v>420</v>
+        <v>399</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B121">
         <f t="shared" si="1"/>
@@ -4059,22 +4027,21 @@
         <v>8</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E121" s="1">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="F121" s="1">
-        <v>421</v>
+        <v>400</v>
       </c>
       <c r="G121" s="1">
-        <f t="shared" si="2"/>
-        <v>470</v>
+        <v>402</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B122">
         <f t="shared" si="1"/>
@@ -4084,42 +4051,112 @@
         <v>8</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E122" s="1">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F122" s="1">
-        <v>471</v>
+        <v>403</v>
       </c>
       <c r="G122" s="1">
-        <f t="shared" si="2"/>
-        <v>502</v>
+        <v>422</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>255</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D123" t="s">
+        <v>255</v>
+      </c>
+      <c r="E123" s="1">
+        <v>1</v>
+      </c>
+      <c r="F123" s="1">
+        <v>423</v>
+      </c>
+      <c r="G123" s="1">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>248</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C124" t="s">
+        <v>8</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E124" s="1">
+        <v>50</v>
+      </c>
+      <c r="F124" s="1">
+        <v>424</v>
+      </c>
+      <c r="G124" s="1">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>249</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C125" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E125" s="1">
+        <v>32</v>
+      </c>
+      <c r="F125" s="1">
+        <v>474</v>
+      </c>
+      <c r="G125" s="1">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>251</v>
       </c>
-      <c r="B123">
-        <f t="shared" si="1"/>
-        <v>1284</v>
-      </c>
-      <c r="C123" t="s">
-        <v>8</v>
-      </c>
-      <c r="D123" s="1" t="s">
+      <c r="B126">
+        <f t="shared" si="1"/>
+        <v>1934</v>
+      </c>
+      <c r="C126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E123" s="1">
-        <v>781</v>
-      </c>
-      <c r="F123" s="1">
-        <v>503</v>
-      </c>
-      <c r="G123" s="1">
-        <f t="shared" si="2"/>
-        <v>1283</v>
+      <c r="E126">
+        <v>1428</v>
+      </c>
+      <c r="F126">
+        <v>506</v>
+      </c>
+      <c r="G126">
+        <v>1933</v>
       </c>
     </row>
   </sheetData>

</xml_diff>